<commit_message>
added necessary sheets for prototype
</commit_message>
<xml_diff>
--- a/Project_Prototype.xlsx
+++ b/Project_Prototype.xlsx
@@ -5,15 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\EduQuant-Project-Data-Focused-Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\amtalb\95888\group_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59B08806-BFF9-4C63-A177-7B856B9E75E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3369A8C-A0C6-427D-8157-91537D008A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="5028" windowWidth="23256" windowHeight="12576" xr2:uid="{B1DF6E76-0021-402F-B486-123D3224DB04}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="8" xr2:uid="{B1DF6E76-0021-402F-B486-123D3224DB04}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="NASDAQ - Raw" sheetId="2" r:id="rId2"/>
+    <sheet name="NASDAQ - Clean" sheetId="3" r:id="rId3"/>
+    <sheet name="NYSE - Raw" sheetId="4" r:id="rId4"/>
+    <sheet name="NYSE - Clean" sheetId="5" r:id="rId5"/>
+    <sheet name="SEC Quarterly - Raw" sheetId="6" r:id="rId6"/>
+    <sheet name="SEC Quarterly - Clean" sheetId="7" r:id="rId7"/>
+    <sheet name="CNN - Raw" sheetId="8" r:id="rId8"/>
+    <sheet name="CNN - Clean" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -382,9 +390,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC69D75-E446-4C1C-9FE1-A74C0BCF07A8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8BEDED-576A-460D-9769-E72139996DAF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207DF5C3-470E-468E-9E72-1ADD81D0283E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EA417A-E125-4842-98A6-DBA604F56E25}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC0EFC3-4EE1-4F01-B513-BAFA36E3F73C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24405389-8B79-48B8-AFF3-6B6B0CD77457}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECB349D-8784-4BA9-BD1C-BB1E7353A97E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A55E7F9-4853-4BFF-9C82-E89C254AB123}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB07DCBF-29CC-4D2E-9AB8-83F2AB2D6BE2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="CC1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add List of Companies to Prototype
</commit_message>
<xml_diff>
--- a/Project_Prototype.xlsx
+++ b/Project_Prototype.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\amtalb\95888\group_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\EduQuant-Project-Data-Focused-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3369A8C-A0C6-427D-8157-91537D008A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3483BC-B19D-455C-94AA-517DBB0BD5E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="8" xr2:uid="{B1DF6E76-0021-402F-B486-123D3224DB04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B1DF6E76-0021-402F-B486-123D3224DB04}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="NASDAQ - Raw" sheetId="2" r:id="rId2"/>
-    <sheet name="NASDAQ - Clean" sheetId="3" r:id="rId3"/>
-    <sheet name="NYSE - Raw" sheetId="4" r:id="rId4"/>
-    <sheet name="NYSE - Clean" sheetId="5" r:id="rId5"/>
-    <sheet name="SEC Quarterly - Raw" sheetId="6" r:id="rId6"/>
-    <sheet name="SEC Quarterly - Clean" sheetId="7" r:id="rId7"/>
-    <sheet name="CNN - Raw" sheetId="8" r:id="rId8"/>
-    <sheet name="CNN - Clean" sheetId="9" r:id="rId9"/>
+    <sheet name="Company List" sheetId="10" r:id="rId2"/>
+    <sheet name="NASDAQ - Raw" sheetId="2" r:id="rId3"/>
+    <sheet name="NASDAQ - Clean" sheetId="3" r:id="rId4"/>
+    <sheet name="NYSE - Raw" sheetId="4" r:id="rId5"/>
+    <sheet name="NYSE - Clean" sheetId="5" r:id="rId6"/>
+    <sheet name="SEC Quarterly - Raw" sheetId="6" r:id="rId7"/>
+    <sheet name="SEC Quarterly - Clean" sheetId="7" r:id="rId8"/>
+    <sheet name="CNN - Raw" sheetId="8" r:id="rId9"/>
+    <sheet name="CNN - Clean" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,6 +42,344 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+  <si>
+    <t>Company ID</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Stock Code</t>
+  </si>
+  <si>
+    <t>APPLE INC.</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>ADOBE INC.</t>
+  </si>
+  <si>
+    <t>ADBE</t>
+  </si>
+  <si>
+    <t>ANALOG DEVICES CMN</t>
+  </si>
+  <si>
+    <t>ADI</t>
+  </si>
+  <si>
+    <t>AUTODESK INC</t>
+  </si>
+  <si>
+    <t>ADSK</t>
+  </si>
+  <si>
+    <t>APPLIED MATERIALS</t>
+  </si>
+  <si>
+    <t>AMAT</t>
+  </si>
+  <si>
+    <t>ADV MICRO DEVICES</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>ANSYS INC</t>
+  </si>
+  <si>
+    <t>ANSS</t>
+  </si>
+  <si>
+    <t>ASML HLDG NY REG</t>
+  </si>
+  <si>
+    <t>ASML</t>
+  </si>
+  <si>
+    <t>BROADCOM INC.</t>
+  </si>
+  <si>
+    <t>AVGO</t>
+  </si>
+  <si>
+    <t>BAIDU, INC.</t>
+  </si>
+  <si>
+    <t>BIDU</t>
+  </si>
+  <si>
+    <t>CADENCE DESIGN SYS</t>
+  </si>
+  <si>
+    <t>CDNS</t>
+  </si>
+  <si>
+    <t>CDW CORPORATION</t>
+  </si>
+  <si>
+    <t>CDW</t>
+  </si>
+  <si>
+    <t>CERNER CORP</t>
+  </si>
+  <si>
+    <t>CERN</t>
+  </si>
+  <si>
+    <t>CHECK POINT SOFTWARE</t>
+  </si>
+  <si>
+    <t>CHKP</t>
+  </si>
+  <si>
+    <t>CISCO SYSTEMS INC</t>
+  </si>
+  <si>
+    <t>CSCO</t>
+  </si>
+  <si>
+    <t>COGNIZANT TECH SOL</t>
+  </si>
+  <si>
+    <t>CTSH</t>
+  </si>
+  <si>
+    <t>CITRIX SYSTEMS INC</t>
+  </si>
+  <si>
+    <t>CTXS</t>
+  </si>
+  <si>
+    <t>DOCUSIGN, INC. CMN</t>
+  </si>
+  <si>
+    <t>DOCU</t>
+  </si>
+  <si>
+    <t>FACEBOOK INC</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>ALPHABET CL C CAP</t>
+  </si>
+  <si>
+    <t>GOOG</t>
+  </si>
+  <si>
+    <t>ALPHABET CL A CMN</t>
+  </si>
+  <si>
+    <t>GOOGL</t>
+  </si>
+  <si>
+    <t>INTEL CORP</t>
+  </si>
+  <si>
+    <t>INTC</t>
+  </si>
+  <si>
+    <t>INTUIT INC</t>
+  </si>
+  <si>
+    <t>INTU</t>
+  </si>
+  <si>
+    <t>KLA CP CMN STK</t>
+  </si>
+  <si>
+    <t>KLAC</t>
+  </si>
+  <si>
+    <t>LAM RESEARCH CORP</t>
+  </si>
+  <si>
+    <t>LRCX</t>
+  </si>
+  <si>
+    <t>MICROCHIP TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>MCHP</t>
+  </si>
+  <si>
+    <t>MICROSOFT CORP</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>MICRON TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>MAXIM INTEGRATED</t>
+  </si>
+  <si>
+    <t>MXIM</t>
+  </si>
+  <si>
+    <t>NETEASE INC ADS</t>
+  </si>
+  <si>
+    <t>NTES</t>
+  </si>
+  <si>
+    <t>NVIDIA CORPORATION</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>NXP SEMICONDUCTORS</t>
+  </si>
+  <si>
+    <t>NXPI</t>
+  </si>
+  <si>
+    <t>QUALCOMM INC</t>
+  </si>
+  <si>
+    <t>QCOM</t>
+  </si>
+  <si>
+    <t>SYNOPSYS, INC.</t>
+  </si>
+  <si>
+    <t>SNPS</t>
+  </si>
+  <si>
+    <t>SPLUNK INC.</t>
+  </si>
+  <si>
+    <t>SPLK</t>
+  </si>
+  <si>
+    <t>SKYWORKS SOLUTIONS</t>
+  </si>
+  <si>
+    <t>SWKS</t>
+  </si>
+  <si>
+    <t>TEXAS INSTRUMENTS</t>
+  </si>
+  <si>
+    <t>TXN</t>
+  </si>
+  <si>
+    <t>VERISIGN, INC.</t>
+  </si>
+  <si>
+    <t>VRSN</t>
+  </si>
+  <si>
+    <t>WORKDAY INC CL A</t>
+  </si>
+  <si>
+    <t>WDAY</t>
+  </si>
+  <si>
+    <t>WESTERN DIGITAL CP</t>
+  </si>
+  <si>
+    <t>WDC</t>
+  </si>
+  <si>
+    <t>XILINX, INC.</t>
+  </si>
+  <si>
+    <t>XLNX</t>
+  </si>
+  <si>
+    <t>Alibaba Group holding Limited</t>
+  </si>
+  <si>
+    <t>BABA</t>
+  </si>
+  <si>
+    <t>Tesla, Inc.</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>salesforce.com, inc.</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>PayPal Holdings, Inc.</t>
+  </si>
+  <si>
+    <t>PYPL</t>
+  </si>
+  <si>
+    <t>Activision Blizzard, Inc.</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
+    <t>Electronic Arts Ind.</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>Match Group, Inc.</t>
+  </si>
+  <si>
+    <t>MTCH</t>
+  </si>
+  <si>
+    <t>Zillow Group, Inc.</t>
+  </si>
+  <si>
+    <t>ZG</t>
+  </si>
+  <si>
+    <t>The Trade Desk, Inc.</t>
+  </si>
+  <si>
+    <t>TTD</t>
+  </si>
+  <si>
+    <t>Yelp Inc.</t>
+  </si>
+  <si>
+    <t>TELP</t>
+  </si>
+  <si>
+    <t>TiVo Corporation</t>
+  </si>
+  <si>
+    <t>TIVO</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>AMZN</t>
+  </si>
+  <si>
+    <t>Taiwan Semiconductor Manufacturing</t>
+  </si>
+  <si>
+    <t>TSM</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -52,12 +391,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,13 +417,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -392,103 +746,729 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB07DCBF-29CC-4D2E-9AB8-83F2AB2D6BE2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="CC1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7D50FD-E17C-492B-AC7C-F81E02DB1A3C}">
+  <dimension ref="A1:C55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8BEDED-576A-460D-9769-E72139996DAF}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207DF5C3-470E-468E-9E72-1ADD81D0283E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EA417A-E125-4842-98A6-DBA604F56E25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207DF5C3-470E-468E-9E72-1ADD81D0283E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC0EFC3-4EE1-4F01-B513-BAFA36E3F73C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EA417A-E125-4842-98A6-DBA604F56E25}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24405389-8B79-48B8-AFF3-6B6B0CD77457}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC0EFC3-4EE1-4F01-B513-BAFA36E3F73C}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECB349D-8784-4BA9-BD1C-BB1E7353A97E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24405389-8B79-48B8-AFF3-6B6B0CD77457}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A55E7F9-4853-4BFF-9C82-E89C254AB123}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECB349D-8784-4BA9-BD1C-BB1E7353A97E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB07DCBF-29CC-4D2E-9AB8-83F2AB2D6BE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A55E7F9-4853-4BFF-9C82-E89C254AB123}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CC1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>